<commit_message>
Adiciona medidas de rotação e translação a dados
</commit_message>
<xml_diff>
--- a/dados/medidas_sistema_solar.xlsx
+++ b/dados/medidas_sistema_solar.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Planetas e Sol" sheetId="1" state="visible" r:id="rId2"/>
@@ -320,7 +320,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -331,6 +331,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -350,23 +354,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1:I10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.4183673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="28.25"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9948979591837"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="27.9438775510204"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -455,6 +457,29 @@
       <c r="I3" s="2" t="n">
         <v>88</v>
       </c>
+      <c r="J3" s="0" t="n">
+        <f aca="false">ROUND(LOG(I3,10), 1)</f>
+        <v>1.9</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <f aca="false">ROUND(EXP(J3),2)</f>
+        <v>6.69</v>
+      </c>
+      <c r="L3" s="2" t="n">
+        <v>58</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <f aca="false">L3*10</f>
+        <v>580</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <f aca="false">LOG10(M3)</f>
+        <v>2.76342799356294</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <f aca="false">ROUND(EXP(N3),2)</f>
+        <v>15.85</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -484,6 +509,29 @@
       <c r="I4" s="2" t="n">
         <v>224.7</v>
       </c>
+      <c r="J4" s="0" t="n">
+        <f aca="false">ROUND(LOG(I4,10), 1)</f>
+        <v>2.4</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <f aca="false">ROUND(EXP(J4),2)</f>
+        <v>11.02</v>
+      </c>
+      <c r="L4" s="2" t="n">
+        <v>243.025</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <f aca="false">L4*10</f>
+        <v>2430.25</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <f aca="false">LOG10(M4)</f>
+        <v>3.38565095180234</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <f aca="false">ROUND(EXP(N4),2)</f>
+        <v>29.54</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -513,6 +561,29 @@
       <c r="I5" s="2" t="n">
         <v>365.2</v>
       </c>
+      <c r="J5" s="0" t="n">
+        <f aca="false">ROUND(LOG(I5,10), 1)</f>
+        <v>2.6</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <f aca="false">ROUND(EXP(J5),2)</f>
+        <v>13.46</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <f aca="false">L5*10</f>
+        <v>10</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <f aca="false">LOG10(M5)</f>
+        <v>1</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <f aca="false">ROUND(EXP(N5),2)</f>
+        <v>2.72</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
@@ -542,6 +613,29 @@
       <c r="I6" s="2" t="n">
         <v>687</v>
       </c>
+      <c r="J6" s="0" t="n">
+        <f aca="false">ROUND(LOG(I6,10), 1)</f>
+        <v>2.8</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <f aca="false">ROUND(EXP(J6),2)</f>
+        <v>16.44</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <f aca="false">L6*10</f>
+        <v>10</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <f aca="false">LOG10(M6)</f>
+        <v>1</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <f aca="false">ROUND(EXP(N6),2)</f>
+        <v>2.72</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -571,6 +665,29 @@
       <c r="I7" s="2" t="n">
         <v>4332</v>
       </c>
+      <c r="J7" s="0" t="n">
+        <f aca="false">ROUND(LOG(I7,10), 1)</f>
+        <v>3.6</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <f aca="false">ROUND(EXP(J7),2)</f>
+        <v>36.6</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <f aca="false">L7*10</f>
+        <v>3.33</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <f aca="false">LOG10(M7)</f>
+        <v>0.52244423350632</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <f aca="false">ROUND(EXP(N7),2)</f>
+        <v>1.69</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -600,6 +717,29 @@
       <c r="I8" s="2" t="n">
         <v>10760</v>
       </c>
+      <c r="J8" s="0" t="n">
+        <f aca="false">ROUND(LOG(I8,10), 1)</f>
+        <v>4</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <f aca="false">ROUND(EXP(J8),2)</f>
+        <v>54.6</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <f aca="false">L8*10</f>
+        <v>4</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <f aca="false">LOG10(M8)</f>
+        <v>0.602059991327962</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <f aca="false">ROUND(EXP(N8),2)</f>
+        <v>1.83</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
@@ -629,6 +769,29 @@
       <c r="I9" s="2" t="n">
         <v>30700</v>
       </c>
+      <c r="J9" s="0" t="n">
+        <f aca="false">ROUND(LOG(I9,10), 1)</f>
+        <v>4.5</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <f aca="false">ROUND(EXP(J9),2)</f>
+        <v>90.02</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <f aca="false">L9*10</f>
+        <v>7.1</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <f aca="false">LOG10(M9)</f>
+        <v>0.851258348719075</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <f aca="false">ROUND(EXP(N9),2)</f>
+        <v>2.34</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
@@ -658,20 +821,68 @@
       <c r="I10" s="2" t="n">
         <v>60200</v>
       </c>
+      <c r="J10" s="0" t="n">
+        <f aca="false">ROUND(LOG(I10,10), 1)</f>
+        <v>4.8</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <f aca="false">ROUND(EXP(J10),2)</f>
+        <v>121.51</v>
+      </c>
+      <c r="L10" s="2" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <f aca="false">L10*10</f>
+        <v>6.7</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <f aca="false">LOG10(M10)</f>
+        <v>0.826074802700826</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <f aca="false">ROUND(EXP(N10),2)</f>
+        <v>2.28</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I11" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <f aca="false">ROUND(LOG(I11,10), 1)</f>
+        <v>1.4</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <f aca="false">ROUND(EXP(J11),2)</f>
+        <v>4.06</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="I12" s="0" t="n">
+        <f aca="false">75*365</f>
+        <v>27375</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <f aca="false">ROUND(LOG(I12,10), 1)</f>
+        <v>4.4</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <f aca="false">ROUND(EXP(J12),2)</f>
+        <v>81.45</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -696,16 +907,14 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="1" sqref="I1:I10 F2"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="1" sqref="I13 F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -767,21 +976,17 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="1" sqref="I1:I10 D17"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="1" sqref="I13 D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.0255102040816"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.1836734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.8469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1350,13 +1555,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="I1:I10 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="I13 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1376,13 +1578,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="I1:I10 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="I13 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1402,13 +1601,12 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="I1:I10 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="I13 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1470,13 +1668,10 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="1" sqref="I1:I10 E4"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="1" sqref="I13 E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1557,17 +1752,15 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="I1:I10 A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="I13 A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.25"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.44897959183673"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1689,14 +1882,12 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="1" sqref="I1:I10 G13"/>
+      <selection pane="topLeft" activeCell="G13" activeCellId="1" sqref="I13 G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.5"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.9591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1838,15 +2029,13 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="1" sqref="I1:I10 A7"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="1" sqref="I13 A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.6377551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.0969387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>